<commit_message>
Cambios para GitHub 👩‍💻
</commit_message>
<xml_diff>
--- a/XLSX Version 3/identificacion.xlsx
+++ b/XLSX Version 3/identificacion.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcastilloaraujo/tucertificado.co/XLSX Prueba Beta 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcastilloaraujo/tucertificado.co/XLSX Version 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C26975-F745-7E48-B95E-798A00BD758D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67F1674-BCD5-CE4D-9142-B413D32FCE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16360" yWindow="1000" windowWidth="18960" windowHeight="15760" xr2:uid="{D050B619-DE5B-3344-B5B8-1D673D1B626A}"/>
+    <workbookView xWindow="9840" yWindow="880" windowWidth="18960" windowHeight="15760" xr2:uid="{D050B619-DE5B-3344-B5B8-1D673D1B626A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$B$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$B$4</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>GLORIA PATRICIA SARMIENTO AVELLANEDA</t>
   </si>
@@ -48,93 +48,6 @@
   </si>
   <si>
     <t>NICOL ALEJANDRA MACHETE VILLAMIL</t>
-  </si>
-  <si>
-    <t>JENNIFER ALEXANDRA CASTRO RODRIGUEZ</t>
-  </si>
-  <si>
-    <t>ANGIE KATHERINE ROBAYO ANGEL</t>
-  </si>
-  <si>
-    <t>JEISON STIVEN RIVERA ORTIZ</t>
-  </si>
-  <si>
-    <t>EMILCE AHUMADA PULIDO</t>
-  </si>
-  <si>
-    <t>LADY LORENA MONTAÑO BERNAL</t>
-  </si>
-  <si>
-    <t>JONATHAN FELIPE AREVALO BUSTOS</t>
-  </si>
-  <si>
-    <t>HEIDY MICHEL ALVAREZ CAMBEROS</t>
-  </si>
-  <si>
-    <t>KAROL DAYANA ROJAS QUIROGA</t>
-  </si>
-  <si>
-    <t>JUAN DAVID PEÑA PINILLA</t>
-  </si>
-  <si>
-    <t>FREDY YAIR CAICEDO MONTAÑO</t>
-  </si>
-  <si>
-    <t>FABIAN CASTIBLANCO CASTIBLANCO</t>
-  </si>
-  <si>
-    <t>BEATRIZ ALAPE TAPIA</t>
-  </si>
-  <si>
-    <t>DEISY TATIANA SUSA PACHON</t>
-  </si>
-  <si>
-    <t>CRISTIAN ALEJANDRO RODRIGUEZ RODRIGUEZ</t>
-  </si>
-  <si>
-    <t>LUIS FRANCISCO TORRES PAIBA</t>
-  </si>
-  <si>
-    <t>JUAN DAVID CABRA MURCIA</t>
-  </si>
-  <si>
-    <t>CARLOS ALFONSO DELGADO SALAZAR</t>
-  </si>
-  <si>
-    <t>JENNSI DAYANA SUAREZ PAEZ</t>
-  </si>
-  <si>
-    <t>EDUAR ESTIBEN GARZON FANDIÑO</t>
-  </si>
-  <si>
-    <t>LINA YULIETH BALLESTEROS PACHÓN</t>
-  </si>
-  <si>
-    <t>JUAN GUILLERMO SIERRA POVEDA</t>
-  </si>
-  <si>
-    <t>YEISON DAVID AHUMADA AHUMADA</t>
-  </si>
-  <si>
-    <t>CRISTIAN YESID MOLINA BELLO</t>
-  </si>
-  <si>
-    <t>BRAYAN FERNANDO MURCIA CORDOBA</t>
-  </si>
-  <si>
-    <t>SHARON ARIADNA RINCON GUERRERO</t>
-  </si>
-  <si>
-    <t>NIDIA YANETH FORERO HURTADO</t>
-  </si>
-  <si>
-    <t>YULIETH STHEPHANIA SANTANA NIETO</t>
-  </si>
-  <si>
-    <t>KAROL XIMENNA AGUILAR GUZMÁN</t>
-  </si>
-  <si>
-    <t>MAIRA TATIANA QUIROGA PERALTA</t>
   </si>
   <si>
     <t>Nombre Completo</t>
@@ -255,9 +168,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -295,7 +208,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -401,7 +314,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -543,7 +456,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E34D78B5-9DF0-904A-B622-7EAC4B92510C}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,10 +478,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -595,240 +508,8 @@
         <v>1077112200</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1076651599</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1077112046</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1007782633</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1075679552</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1074888285</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1053325410</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1074958328</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1072364208</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1077112387</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1003922264</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1003474860</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2">
-        <v>28870080</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2">
-        <v>1076666636</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1003699095</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1077340063</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1077340246</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2">
-        <v>1006814825</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1007696075</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="2">
-        <v>1076649174</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="2">
-        <v>1077112267</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="2">
-        <v>1021394841</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="2">
-        <v>1077112099</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="2">
-        <v>1076646051</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="2">
-        <v>1001175069</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="2">
-        <v>1002740429</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="2">
-        <v>1007467475</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="2">
-        <v>1077112367</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="2">
-        <v>1003474825</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="2">
-        <v>1003909904</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:B33" xr:uid="{E34D78B5-9DF0-904A-B622-7EAC4B92510C}"/>
+  <autoFilter ref="A1:B4" xr:uid="{E34D78B5-9DF0-904A-B622-7EAC4B92510C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>